<commit_message>
Redesign analysis detail page to match HTML prototype
- Replace single-panel layout with two-panel IC memo format (7 sections + property card)
- Fix Tailwind v4 color tokens: use hardcoded hex in @theme inline for opacity modifier support
- Fix body font from Arial to Inter; remove antialiased for correct font weight rendering
- Add new components: AnalysisHeader, KeyMetricsDashboard, CashFlowChart, NOIComparison, PropertyCard, RiskDot, DownloadBar, AnalysisLoadingState

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/LoopMagic Template.xlsx
+++ b/templates/LoopMagic Template.xlsx
@@ -2,84 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etyensegal/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etyensegal/loopmagic/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304E620A-4D2E-D84F-9BD8-3A49CDBE14A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E12FFC-C7FD-8745-A1D6-C316838D8271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17820" xr2:uid="{2A18638E-C092-2644-89A0-5EEACC533054}"/>
+    <workbookView xWindow="4640" yWindow="660" windowWidth="25600" windowHeight="17820" xr2:uid="{2A18638E-C092-2644-89A0-5EEACC533054}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition Model" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-    <externalReference r:id="rId3"/>
-    <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
-    <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
-    <externalReference r:id="rId9"/>
-    <externalReference r:id="rId10"/>
-    <externalReference r:id="rId11"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="__123Graph_A" hidden="1">[1]P!#REF!</definedName>
-    <definedName name="__123Graph_AChart1" hidden="1">[1]P!#REF!</definedName>
-    <definedName name="__123Graph_ACurrent" hidden="1">[1]P!#REF!</definedName>
-    <definedName name="__123Graph_AGATHERING" hidden="1">[2]COC!#REF!</definedName>
-    <definedName name="__123Graph_B" hidden="1">[3]XOM!#REF!</definedName>
-    <definedName name="__123Graph_BSPREADS" hidden="1">[4]TSO!#REF!</definedName>
-    <definedName name="__123Graph_X" hidden="1">[3]XOM!#REF!</definedName>
-    <definedName name="__123Graph_XChart1" hidden="1">[5]P!$R$29:$AK$29</definedName>
-    <definedName name="__123Graph_XCurrent" hidden="1">[5]P!$R$29:$AK$29</definedName>
-    <definedName name="__123Graph_XGATHERING" hidden="1">[2]COC!#REF!</definedName>
-    <definedName name="__FDS_HYPERLINK_TOGGLE_STATE__" hidden="1">"ON"</definedName>
-    <definedName name="_10__123Graph_BGASOLINE\_2" hidden="1">[4]TSO!#REF!</definedName>
-    <definedName name="_12__123Graph_XGASOLINE\_2" hidden="1">[4]TSO!#REF!</definedName>
-    <definedName name="_13__123Graph_XLIQUIDS" hidden="1">[5]P!$R$29:$AK$29</definedName>
-    <definedName name="_15__123Graph_XOP_COSTS" hidden="1">[4]TSO!#REF!</definedName>
-    <definedName name="_16__123Graph_XR_M_MARG" hidden="1">[5]P!$R$29:$AK$29</definedName>
-    <definedName name="_2__123Graph_AGASOLINE\_2" hidden="1">[4]TSO!#REF!</definedName>
-    <definedName name="_4__123Graph_ALIQUIDS" hidden="1">[6]COP!#REF!</definedName>
-    <definedName name="_6__123Graph_AOP_COSTS" hidden="1">[4]TSO!#REF!</definedName>
-    <definedName name="_8__123Graph_AR_M_MARG" hidden="1">[1]P!#REF!</definedName>
-    <definedName name="_bdm.27A67F90C7C644ABA5AEE92323AE8841.edm" hidden="1">'[7]New Source Charts'!$A:$IV</definedName>
-    <definedName name="_bdm.2F994D6394314D65966806B0027B7ED0.edm" hidden="1">[8]Plants!$A:$IV</definedName>
-    <definedName name="_bdm.3D459AB342314C87AF28EE2023B5B5D2.edm" hidden="1">[7]Modelware!$A:$IV</definedName>
-    <definedName name="_bdm.4AF7B9937D644F5F89369844785EF279.edm" hidden="1">[8]VeraSun!$A:$IV</definedName>
-    <definedName name="_bdm.51DB0A22AC534FDAAE0186334B0F5CC7.edm" hidden="1">#REF!</definedName>
-    <definedName name="_bdm.556C0F41CE9F461F93C646A4B737FE37.edm" hidden="1">'[8]Forecast Change'!$A:$IV</definedName>
-    <definedName name="_bdm.6A05919F37494F38ACE807AC7DE0AF1C.edm" hidden="1">#REF!</definedName>
-    <definedName name="_bdm.6C3127543B3B4F248937555D27DB740A.edm" hidden="1">[9]PXP!$A:$IV</definedName>
-    <definedName name="_bdm.80AA8F96F3EC41DCA0719BEA7F3C72E4.edm" hidden="1">'[7]Segment ROCE'!$A:$IV</definedName>
-    <definedName name="_bdm.A167D12DAE3248FDB8A1CC583636203E.edm" hidden="1">#REF!</definedName>
-    <definedName name="_bdm.AA6C2D22BE3E4F2895813DA1409C2ED5.edm" hidden="1">[7]BS!$A:$IV</definedName>
-    <definedName name="_bdm.B187957A40074E88B68BA9B13084EB53.edm" hidden="1">[7]COP!$A:$IV</definedName>
-    <definedName name="_bdm.B2DA56CA5AA740E6AFBE3497C6982B4B.edm" hidden="1">'[7]R&amp;MIS'!$A:$IV</definedName>
-    <definedName name="_bdm.BC1DD9D4902146ED81E611A5BC71C3AD.edm" hidden="1">[8]INPUTS!$A:$IV</definedName>
-    <definedName name="_bdm.FD343515BA234434BE623D650D6B8A99.edm" hidden="1">'[7]E&amp;P Growth &amp; Returns'!$A:$IV</definedName>
     <definedName name="abc" hidden="1">{"Cover",#N/A,FALSE,"Cover";"Summary",#N/A,FALSE,"Summarpage";"Assumptions",#N/A,FALSE,"Assumptions";"Earnings",#N/A,FALSE,"Earnings";"CF Oper.",#N/A,FALSE,"Earnings";"Balance Sheet",#N/A,FALSE,"balance";"Cash Flow",#N/A,FALSE,"cash flow";"Paper Production",#N/A,FALSE,"Paper";"Paper Earnings",#N/A,FALSE,"Paper";"Wood Production",#N/A,FALSE,"Wood Products";"Wood Earnings",#N/A,FALSE,"Wood Products";"Pulp Production",#N/A,FALSE,"Pulp";"Pulp Earnings",#N/A,FALSE,"Pulp"}</definedName>
-    <definedName name="beta_observed">#REF!</definedName>
-    <definedName name="beta_unlev_comps">#REF!</definedName>
-    <definedName name="conversionfactor">'[10]E&amp;P'!$D$6</definedName>
-    <definedName name="convfactor">#REF!</definedName>
-    <definedName name="costdebtfirm">#REF!</definedName>
-    <definedName name="costequity">#REF!</definedName>
-    <definedName name="days_per_year">#REF!</definedName>
-    <definedName name="debt">#REF!</definedName>
-    <definedName name="debt_weight">#REF!</definedName>
-    <definedName name="market_equity">#REF!</definedName>
-    <definedName name="relevered_beta">#REF!</definedName>
-    <definedName name="risk_free_rate">#REF!</definedName>
-    <definedName name="risk_premium">#REF!</definedName>
-    <definedName name="stubyear">#REF!</definedName>
-    <definedName name="totalcap">#REF!</definedName>
-    <definedName name="wacc">#REF!</definedName>
     <definedName name="wrn.2._.pagers." hidden="1">{"Cover",#N/A,FALSE,"Cover";"Summary",#N/A,FALSE,"Summarpage"}</definedName>
     <definedName name="wrn.allpages." hidden="1">{#N/A,#N/A,TRUE,"Historicals";#N/A,#N/A,TRUE,"Charts";#N/A,#N/A,TRUE,"Forecasts"}</definedName>
     <definedName name="wrn.Complete." hidden="1">{"Cover",#N/A,FALSE,"Cover";"Summary",#N/A,FALSE,"Summarpage";"Assumptions",#N/A,FALSE,"Assumptions";"Earnings",#N/A,FALSE,"Earnings";"CF Oper.",#N/A,FALSE,"Earnings";"Balance Sheet",#N/A,FALSE,"balance";"Cash Flow",#N/A,FALSE,"cash flow";"Paper Production",#N/A,FALSE,"Paper";"Paper Earnings",#N/A,FALSE,"Paper";"Wood Production",#N/A,FALSE,"Wood Products";"Wood Earnings",#N/A,FALSE,"Wood Products";"Pulp Production",#N/A,FALSE,"Pulp";"Pulp Earnings",#N/A,FALSE,"Pulp"}</definedName>
@@ -111,30 +48,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
   <si>
     <t>CRE ACQUISITION MODEL</t>
   </si>
@@ -422,8 +337,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;\(&quot;$&quot;#,##0\);&quot;-&quot;"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
@@ -646,7 +562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -708,12 +624,9 @@
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -737,22 +650,16 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="5" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="5" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="5" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="5" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="5" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="5" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="5" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="5" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,914 +676,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="P"/>
-      <sheetName val="BS"/>
-      <sheetName val="Variance"/>
-      <sheetName val="Segment ROCE"/>
-      <sheetName val="Capex"/>
-      <sheetName val="E&amp;P"/>
-      <sheetName val="Relative"/>
-      <sheetName val="ROGIC"/>
-      <sheetName val="NEPS"/>
-      <sheetName val="Hamaca"/>
-      <sheetName val="Bohai"/>
-      <sheetName val="Bayu Undan"/>
-      <sheetName val="R&amp;M"/>
-      <sheetName val="GPM"/>
-      <sheetName val="ARCO - Alaska"/>
-      <sheetName val="RefineryMaint"/>
-      <sheetName val="TOSCO"/>
-      <sheetName val="Reserves"/>
-      <sheetName val="WACC"/>
-      <sheetName val="Valuation"/>
-      <sheetName val="NAV"/>
-      <sheetName val="Chemical JV"/>
-      <sheetName val="Chems"/>
-      <sheetName val="EKOFISK"/>
-      <sheetName val="PUDS"/>
-      <sheetName val="GE Data"/>
-      <sheetName val="MainCode"/>
-      <sheetName val="NY UPLOAD"/>
-      <sheetName val="NY UPLOAD shadow"/>
-      <sheetName val="Disclaimer"/>
-      <sheetName val="Quarterly"/>
-      <sheetName val="IndexInformation"/>
-      <sheetName val="NORM"/>
-      <sheetName val="NY UPLOAD.bak"/>
-      <sheetName val="NY UPLOAD Shadow.bak"/>
-      <sheetName val="Normalized"/>
-      <sheetName val="DDM"/>
-      <sheetName val="B Sheet"/>
-      <sheetName val="Ratios"/>
-      <sheetName val="SOLP"/>
-      <sheetName val="Liquids"/>
-      <sheetName val="charts"/>
-      <sheetName val="Apples-Ratios"/>
-      <sheetName val="IS"/>
-      <sheetName val="Quarterly Data"/>
-      <sheetName val="Debt"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="A-Link Source"/>
-      <sheetName val="IBES"/>
-      <sheetName val="Model"/>
-      <sheetName val="Value-A"/>
-      <sheetName val="US"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Intro"/>
-      <sheetName val="finmodeling"/>
-      <sheetName val="E&amp;P"/>
-      <sheetName val="Price  Deck"/>
-      <sheetName val="E&amp;PIS"/>
-      <sheetName val="CAPEX"/>
-      <sheetName val="Chemicals"/>
-      <sheetName val="BoostToolkitClipBoard2010"/>
-      <sheetName val="Reserves"/>
-      <sheetName val="Hedge"/>
-      <sheetName val="SEC PV 10"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="6">
-          <cell r="D6">
-            <v>6</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="COC"/>
-      <sheetName val="Variance"/>
-      <sheetName val="BS"/>
-      <sheetName val="Capex"/>
-      <sheetName val="ROCE"/>
-      <sheetName val="Corp. "/>
-      <sheetName val="Emerging Bus."/>
-      <sheetName val="NEPS"/>
-      <sheetName val="Quarterly"/>
-      <sheetName val="US E&amp;P"/>
-      <sheetName val="Eu.E&amp;P"/>
-      <sheetName val="Other E&amp;P"/>
-      <sheetName val="P"/>
-      <sheetName val="R&amp;M"/>
-      <sheetName val="COC vs. Wood Mac Prod. Profile"/>
-      <sheetName val="E&amp;P-Conoco"/>
-      <sheetName val="E&amp;P-Total"/>
-      <sheetName val="GOU"/>
-      <sheetName val="PETROZUATA"/>
-      <sheetName val="Lifting_DD&amp;A"/>
-      <sheetName val="PZ2"/>
-      <sheetName val="Corporate ROGIC"/>
-      <sheetName val="WACC"/>
-      <sheetName val="NAV"/>
-      <sheetName val="Reserves"/>
-      <sheetName val="Charts"/>
-      <sheetName val="Debt Cov"/>
-      <sheetName val="NG&amp;GP"/>
-      <sheetName val="LOBO"/>
-      <sheetName val="Pro-Forma Reserves"/>
-      <sheetName val="F&amp;D"/>
-      <sheetName val="Split"/>
-      <sheetName val="GE Data"/>
-      <sheetName val="mStartup"/>
-      <sheetName val="NY UPLOAD"/>
-      <sheetName val="NY UPLOAD shadow"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="XOM"/>
-      <sheetName val="BS"/>
-      <sheetName val="ROCE"/>
-      <sheetName val="Variance"/>
-      <sheetName val="E&amp;P"/>
-      <sheetName val="CapEx"/>
-      <sheetName val="NSOURCE"/>
-      <sheetName val="EE&amp;P"/>
-      <sheetName val="Global E&amp;P Field Percentages"/>
-      <sheetName val="Chems"/>
-      <sheetName val="Realtive"/>
-      <sheetName val="DIVIS"/>
-      <sheetName val="MobilPurchase"/>
-      <sheetName val="MKT"/>
-      <sheetName val="I R&amp;M"/>
-      <sheetName val="R&amp;M"/>
-      <sheetName val="NEPS"/>
-      <sheetName val="ROGIC"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="WACC"/>
-      <sheetName val="Reserves"/>
-      <sheetName val="MainCode"/>
-      <sheetName val="RefineryMaint"/>
-      <sheetName val="GE Data"/>
-      <sheetName val="NY UPLOAD"/>
-      <sheetName val="NY UPLOAD shadow"/>
-      <sheetName val="EPPR."/>
-      <sheetName val="Disclaimer"/>
-      <sheetName val="I.MKT"/>
-      <sheetName val="IndexInformation"/>
-      <sheetName val="Quarterly"/>
-      <sheetName val="NY UPLOAD.bak"/>
-      <sheetName val="NY UPLOAD Shadow.bak"/>
-      <sheetName val="E&amp;P-2"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="OPEBs"/>
-      <sheetName val="DCF"/>
-      <sheetName val="YUKOS"/>
-      <sheetName val="Pensions"/>
-      <sheetName val="DEKA"/>
-      <sheetName val=""/>
-      <sheetName val="mwareTaxoPres"/>
-      <sheetName val="Model_Template"/>
-      <sheetName val="mwareValPrintout"/>
-      <sheetName val="mwarePreview"/>
-      <sheetName val="IS"/>
-      <sheetName val="E&amp;PIS"/>
-      <sheetName val="R&amp;MIS"/>
-      <sheetName val="ChemsIS"/>
-      <sheetName val="Corporate"/>
-      <sheetName val="MODELWARE"/>
-      <sheetName val="ReservesRegion"/>
-      <sheetName val="Share Repurchase"/>
-      <sheetName val="WorkingCapital"/>
-      <sheetName val="R&amp;M ROCE by Region"/>
-      <sheetName val="IR&amp;M"/>
-      <sheetName val="Marketing"/>
-      <sheetName val="US Pension"/>
-      <sheetName val="Intl Pension"/>
-      <sheetName val="A-Link Source"/>
-      <sheetName val="DRC"/>
-      <sheetName val="Q-Link Source"/>
-      <sheetName val="Turnarounds"/>
-      <sheetName val="Global Product Sum"/>
-      <sheetName val="mwareDates"/>
-      <sheetName val="mwareSettings"/>
-      <sheetName val="GҘ Data"/>
-      <sheetName val="ES_x0009_SHOW.INFO_x0005_SPLIT_x0009_ON.WINDOW_x0007_ON"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-      <sheetData sheetId="59" refreshError="1"/>
-      <sheetData sheetId="60" refreshError="1"/>
-      <sheetData sheetId="61" refreshError="1"/>
-      <sheetData sheetId="62" refreshError="1"/>
-      <sheetData sheetId="63" refreshError="1"/>
-      <sheetData sheetId="64" refreshError="1"/>
-      <sheetData sheetId="65" refreshError="1"/>
-      <sheetData sheetId="66" refreshError="1"/>
-      <sheetData sheetId="67" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="TSO"/>
-      <sheetName val="Stats"/>
-      <sheetName val="BS"/>
-      <sheetName val="NORM"/>
-      <sheetName val="ROCE"/>
-      <sheetName val="WACC"/>
-      <sheetName val="Capex"/>
-      <sheetName val="MainCode"/>
-      <sheetName val="BP Acquisition"/>
-      <sheetName val="Golden Eagle"/>
-      <sheetName val="Variance"/>
-      <sheetName val="GE Data"/>
-      <sheetName val="NY UPLOAD"/>
-      <sheetName val="NY UPLOAD Shadow"/>
-      <sheetName val="MWare_Cached"/>
-      <sheetName val="NYMEX"/>
-      <sheetName val="mwareTaxoPres"/>
-      <sheetName val="R-Stats"/>
-      <sheetName val="M-Stats"/>
-      <sheetName val="Debt"/>
-      <sheetName val="ShareRepurchase"/>
-      <sheetName val="mwareValPrintout"/>
-      <sheetName val="mwarePreview"/>
-      <sheetName val="Modelware"/>
-      <sheetName val="Pensions"/>
-      <sheetName val="OPEB"/>
-      <sheetName val="TSOIS"/>
-      <sheetName val="mwareDates"/>
-      <sheetName val="mwareSettings"/>
-      <sheetName val="A-Link Source"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Disclaimer"/>
-      <sheetName val="P"/>
-      <sheetName val="BS"/>
-      <sheetName val="TOSCO"/>
-      <sheetName val="Segment ROCE"/>
-      <sheetName val="ROGIC"/>
-      <sheetName val="E&amp;P"/>
-      <sheetName val="NEPS"/>
-      <sheetName val="RefineryMaint"/>
-      <sheetName val="Hamaca"/>
-      <sheetName val="Bohai"/>
-      <sheetName val="Bayu Undan"/>
-      <sheetName val="R&amp;M"/>
-      <sheetName val="GPM"/>
-      <sheetName val="Variance"/>
-      <sheetName val="ARCO - Alaska"/>
-      <sheetName val="Capex"/>
-      <sheetName val="Reserves"/>
-      <sheetName val="WACC"/>
-      <sheetName val="Valuation"/>
-      <sheetName val="NAV"/>
-      <sheetName val="Chemical JV"/>
-      <sheetName val="Chems"/>
-      <sheetName val="EKOFISK"/>
-      <sheetName val="PUDS"/>
-      <sheetName val="GE Data"/>
-      <sheetName val="IndexInformation"/>
-      <sheetName val="MainCode"/>
-      <sheetName val="NY UPLOAD"/>
-      <sheetName val="NY UPLOAD Shadow"/>
-      <sheetName val="Distribution"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="mwareValPrintout"/>
-      <sheetName val="Summary"/>
-      <sheetName val="mwarePreview"/>
-      <sheetName val="COP"/>
-      <sheetName val="TOTIS"/>
-      <sheetName val="BS"/>
-      <sheetName val="Segment ROCE"/>
-      <sheetName val="Modelware"/>
-      <sheetName val="E&amp;PIS"/>
-      <sheetName val="E&amp;P"/>
-      <sheetName val="R&amp;MIS"/>
-      <sheetName val="NEW SOURCE"/>
-      <sheetName val="CHEMIS"/>
-      <sheetName val="Midstream"/>
-      <sheetName val="ALASKA"/>
-      <sheetName val="Working Cap"/>
-      <sheetName val="Corp"/>
-      <sheetName val="Capex"/>
-      <sheetName val="SYNCRUDE"/>
-      <sheetName val="ShareRepurchase"/>
-      <sheetName val="OP"/>
-      <sheetName val="Debt Schedule"/>
-      <sheetName val="COP_Bear_to_Bull_Chart"/>
-      <sheetName val="Reserves"/>
-      <sheetName val="COP_Bear_to_Bull_Data"/>
-      <sheetName val="COP-EN"/>
-      <sheetName val="COP_Risk-Reward_View_Chart"/>
-      <sheetName val="COP-BR"/>
-      <sheetName val="A-Link Source"/>
-      <sheetName val="COP-BR Update"/>
-      <sheetName val="New Source Charts"/>
-      <sheetName val="LNG"/>
-      <sheetName val="Q-Link Source"/>
-      <sheetName val="mwareTaxoPres"/>
-      <sheetName val="US Pension"/>
-      <sheetName val="Intl Pension"/>
-      <sheetName val="OPEBs"/>
-      <sheetName val="Pension Adjustment"/>
-      <sheetName val="Variance"/>
-      <sheetName val="Admin Pages Follow"/>
-      <sheetName val="E&amp;P Growth &amp; Returns"/>
-      <sheetName val="STRAT"/>
-      <sheetName val="Bayu Undan"/>
-      <sheetName val="R&amp;M"/>
-      <sheetName val="Hamaca"/>
-      <sheetName val="GPM"/>
-      <sheetName val="Global Production Interest"/>
-      <sheetName val="Bohai"/>
-      <sheetName val="Chemical JV"/>
-      <sheetName val="Chems"/>
-      <sheetName val="EKOFISK"/>
-      <sheetName val="PUDS"/>
-      <sheetName val="MainCode"/>
-      <sheetName val="mwareSettings"/>
-      <sheetName val="Global Product Sum"/>
-      <sheetName val="mwareDates"/>
-      <sheetName val="NY UPLOAD shadow"/>
-      <sheetName val="COP - RRV"/>
-      <sheetName val="mwareDates_39111_8204615"/>
-      <sheetName val="MWare_Cached"/>
-      <sheetName val="NewReserves"/>
-      <sheetName val="DEKA"/>
-      <sheetName val="GE Data"/>
-      <sheetName val="NY UPLOAD"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-      <sheetData sheetId="59" refreshError="1"/>
-      <sheetData sheetId="60" refreshError="1"/>
-      <sheetData sheetId="61" refreshError="1"/>
-      <sheetData sheetId="62" refreshError="1"/>
-      <sheetData sheetId="63" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="mwareValPrintout"/>
-      <sheetName val="Summary"/>
-      <sheetName val="mwarePreview"/>
-      <sheetName val="COP"/>
-      <sheetName val="TOTIS"/>
-      <sheetName val="Variance"/>
-      <sheetName val="Segment ROCE"/>
-      <sheetName val="BS"/>
-      <sheetName val="E&amp;PIS"/>
-      <sheetName val="RRV"/>
-      <sheetName val="R&amp;MIS"/>
-      <sheetName val="CHEMIS"/>
-      <sheetName val="E&amp;P"/>
-      <sheetName val="Corp"/>
-      <sheetName val="NEW SOURCE"/>
-      <sheetName val="COP-BR"/>
-      <sheetName val="COP-BR Update"/>
-      <sheetName val="Modelware"/>
-      <sheetName val="Capex"/>
-      <sheetName val="Midstream"/>
-      <sheetName val="Reserves"/>
-      <sheetName val="Working Cap"/>
-      <sheetName val="Debt Schedule"/>
-      <sheetName val="A-Link Source"/>
-      <sheetName val="ShareRepurchase"/>
-      <sheetName val="New Source Charts"/>
-      <sheetName val="LNG"/>
-      <sheetName val="Q-Link Source"/>
-      <sheetName val="mwareTaxoPres"/>
-      <sheetName val="US Pension"/>
-      <sheetName val="Intl Pension"/>
-      <sheetName val="OPEBs"/>
-      <sheetName val="Pension Adjustment"/>
-      <sheetName val="Admin Pages Follow"/>
-      <sheetName val="E&amp;P Growth &amp; Returns"/>
-      <sheetName val="STRAT"/>
-      <sheetName val="Bayu Undan"/>
-      <sheetName val="R&amp;M"/>
-      <sheetName val="Hamaca"/>
-      <sheetName val="GPM"/>
-      <sheetName val="Global Production Interest"/>
-      <sheetName val="Bohai"/>
-      <sheetName val="Chemical JV"/>
-      <sheetName val="Chems"/>
-      <sheetName val="EKOFISK"/>
-      <sheetName val="PUDS"/>
-      <sheetName val="MainCode"/>
-      <sheetName val="mwareDates"/>
-      <sheetName val="mwareSettings"/>
-      <sheetName val="Global Product Sum"/>
-      <sheetName val="NY UPLOAD shadow"/>
-      <sheetName val="P"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Variance (2)"/>
-      <sheetName val="Forecast Change"/>
-      <sheetName val="Variance"/>
-      <sheetName val="INPUTS"/>
-      <sheetName val="VeraSun"/>
-      <sheetName val="DCF"/>
-      <sheetName val="Comps"/>
-      <sheetName val="VE85"/>
-      <sheetName val="Conversions"/>
-      <sheetName val="calc summary"/>
-      <sheetName val="Plants"/>
-      <sheetName val="Risk-Reward_View_Chart"/>
-      <sheetName val="Bear_to_Bull_Chart"/>
-      <sheetName val="Bear_to_Bull_Data"/>
-      <sheetName val="Modelware"/>
-      <sheetName val="mwareDates"/>
-      <sheetName val="mwareSettings"/>
-      <sheetName val="A-Link Source"/>
-      <sheetName val="Val Snapshot"/>
-      <sheetName val="Q-Link Source"/>
-      <sheetName val="DCF Summary"/>
-      <sheetName val="New Source Charts"/>
-      <sheetName val="Segment ROCE"/>
-      <sheetName val="BS"/>
-      <sheetName val="COP"/>
-      <sheetName val="R&amp;MIS"/>
-      <sheetName val="E&amp;P Growth &amp; Returns"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Modelware items"/>
-      <sheetName val="charts"/>
-      <sheetName val="Old_NEW"/>
-      <sheetName val="EPS notes"/>
-      <sheetName val="Est v Act"/>
-      <sheetName val="GUIDANCE"/>
-      <sheetName val="PXP"/>
-      <sheetName val="__FDSCACHE__"/>
-      <sheetName val="Valuation"/>
-      <sheetName val="Hedges"/>
-      <sheetName val="Reserves &amp; Capex"/>
-      <sheetName val="Unbooked Summary"/>
-      <sheetName val="Benchmark Prices"/>
-      <sheetName val="Oil sale split"/>
-      <sheetName val="ASSETS"/>
-      <sheetName val="Basin summary"/>
-      <sheetName val="Pension"/>
-      <sheetName val="Deferred taxes"/>
-      <sheetName val="mwareDates"/>
-      <sheetName val="test"/>
-      <sheetName val="mwareSettings"/>
-      <sheetName val="Plants"/>
-      <sheetName val="VeraSun"/>
-      <sheetName val="Forecast Change"/>
-      <sheetName val="INPUTS"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1998,17 +997,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4DAA48-A4FA-2845-AC46-0123545017E7}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
     <col min="4" max="4" width="26.6640625" customWidth="1"/>
     <col min="5" max="15" width="15.83203125" customWidth="1"/>
   </cols>
@@ -2102,43 +1102,43 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9">
         <f>$B$7*F13*12</f>
-        <v>741600</v>
+        <v>1112400</v>
       </c>
       <c r="G6" s="9">
         <f>$B$7*G13*12</f>
-        <v>763848.00000000012</v>
+        <v>1145772.0000000002</v>
       </c>
       <c r="H6" s="9">
         <f>$B$7*H13*12</f>
-        <v>786763.44000000018</v>
+        <v>1180145.1600000001</v>
       </c>
       <c r="I6" s="9">
         <f>$B$7*I13*12</f>
-        <v>810366.34320000024</v>
+        <v>1215549.5148000005</v>
       </c>
       <c r="J6" s="9">
         <f t="shared" ref="J6:O6" si="0">$B$7*J13*12</f>
-        <v>834677.33349600015</v>
+        <v>1252016.0002440002</v>
       </c>
       <c r="K6" s="9">
         <f t="shared" si="0"/>
-        <v>859717.65350088035</v>
+        <v>1289576.4802513204</v>
       </c>
       <c r="L6" s="9">
         <f t="shared" si="0"/>
-        <v>885509.18310590659</v>
+        <v>1328263.7746588599</v>
       </c>
       <c r="M6" s="9">
         <f t="shared" si="0"/>
-        <v>912074.45859908382</v>
+        <v>1368111.6878986256</v>
       </c>
       <c r="N6" s="9">
         <f t="shared" si="0"/>
-        <v>939436.69235705631</v>
+        <v>1409155.0385355845</v>
       </c>
       <c r="O6" s="10">
         <f t="shared" si="0"/>
-        <v>967619.79312776809</v>
+        <v>1451429.6896916521</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -2146,7 +1146,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="11">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="5" t="s">
@@ -2154,43 +1154,43 @@
       </c>
       <c r="F7" s="9">
         <f>-F6*(1-F12)</f>
-        <v>-111240.00000000001</v>
+        <v>-166860.00000000003</v>
       </c>
       <c r="G7" s="9">
         <f>-G6*(1-G12)</f>
-        <v>-38192.400000000038</v>
+        <v>-57288.600000000064</v>
       </c>
       <c r="H7" s="9">
         <f>-H6*(1-H12)</f>
-        <v>-39338.172000000042</v>
+        <v>-59007.25800000006</v>
       </c>
       <c r="I7" s="9">
         <f>-I6*(1-I12)</f>
-        <v>-40518.31716000005</v>
+        <v>-60777.475740000074</v>
       </c>
       <c r="J7" s="9">
         <f t="shared" ref="J7:N7" si="1">-J6*(1-J12)</f>
-        <v>-41733.866674800047</v>
+        <v>-62600.800012200067</v>
       </c>
       <c r="K7" s="9">
         <f t="shared" si="1"/>
-        <v>-42985.882675044057</v>
+        <v>-64478.824012566074</v>
       </c>
       <c r="L7" s="9">
         <f t="shared" si="1"/>
-        <v>-44275.459155295372</v>
+        <v>-66413.188732943061</v>
       </c>
       <c r="M7" s="9">
         <f t="shared" si="1"/>
-        <v>-45603.72292995423</v>
+        <v>-68405.584394931342</v>
       </c>
       <c r="N7" s="9">
         <f t="shared" si="1"/>
-        <v>-46971.834617852859</v>
+        <v>-70457.751926779281</v>
       </c>
       <c r="O7" s="10">
         <f>-O6*(1-O12)</f>
-        <v>-48380.989656388447</v>
+        <v>-72571.484484582674</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -2206,43 +1206,43 @@
       </c>
       <c r="F8" s="16">
         <f>F6+F7</f>
-        <v>630360</v>
+        <v>945540</v>
       </c>
       <c r="G8" s="16">
         <f>G6+G7</f>
-        <v>725655.60000000009</v>
+        <v>1088483.4000000001</v>
       </c>
       <c r="H8" s="16">
         <f>H6+H7</f>
-        <v>747425.26800000016</v>
+        <v>1121137.902</v>
       </c>
       <c r="I8" s="16">
         <f>I6+I7</f>
-        <v>769848.02604000014</v>
+        <v>1154772.0390600003</v>
       </c>
       <c r="J8" s="16">
         <f t="shared" ref="J8:N8" si="2">J6+J7</f>
-        <v>792943.4668212001</v>
+        <v>1189415.2002318001</v>
       </c>
       <c r="K8" s="16">
         <f t="shared" si="2"/>
-        <v>816731.77082583634</v>
+        <v>1225097.6562387543</v>
       </c>
       <c r="L8" s="16">
         <f t="shared" si="2"/>
-        <v>841233.72395061119</v>
+        <v>1261850.5859259169</v>
       </c>
       <c r="M8" s="16">
         <f t="shared" si="2"/>
-        <v>866470.73566912964</v>
+        <v>1299706.1035036943</v>
       </c>
       <c r="N8" s="16">
         <f t="shared" si="2"/>
-        <v>892464.85773920349</v>
+        <v>1338697.2866088052</v>
       </c>
       <c r="O8" s="17">
         <f>O6+O7</f>
-        <v>919238.80347137968</v>
+        <v>1378858.2052070694</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -2254,43 +1254,43 @@
       </c>
       <c r="F9" s="9">
         <f>$B$37*$B$7*12</f>
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="G9" s="9">
-        <f>F9*(1+$B$38)</f>
-        <v>73800</v>
+        <f t="shared" ref="G9:O9" si="3">F9*(1+$B$38)</f>
+        <v>110699.99999999999</v>
       </c>
       <c r="H9" s="9">
-        <f>G9*(1+$B$38)</f>
-        <v>75645</v>
+        <f t="shared" si="3"/>
+        <v>113467.49999999997</v>
       </c>
       <c r="I9" s="9">
-        <f>H9*(1+$B$38)</f>
-        <v>77536.125</v>
+        <f t="shared" si="3"/>
+        <v>116304.18749999996</v>
       </c>
       <c r="J9" s="9">
-        <f>I9*(1+$B$38)</f>
-        <v>79474.528124999997</v>
+        <f t="shared" si="3"/>
+        <v>119211.79218749994</v>
       </c>
       <c r="K9" s="9">
-        <f>J9*(1+$B$38)</f>
-        <v>81461.391328124984</v>
+        <f t="shared" si="3"/>
+        <v>122192.08699218743</v>
       </c>
       <c r="L9" s="9">
-        <f>K9*(1+$B$38)</f>
-        <v>83497.926111328095</v>
+        <f t="shared" si="3"/>
+        <v>125246.8891669921</v>
       </c>
       <c r="M9" s="9">
-        <f>L9*(1+$B$38)</f>
-        <v>85585.374264111291</v>
+        <f t="shared" si="3"/>
+        <v>128378.06139616689</v>
       </c>
       <c r="N9" s="9">
-        <f>M9*(1+$B$38)</f>
-        <v>87725.00862071407</v>
+        <f t="shared" si="3"/>
+        <v>131587.51293107105</v>
       </c>
       <c r="O9" s="9">
-        <f>N9*(1+$B$38)</f>
-        <v>89918.133836231907</v>
+        <f t="shared" si="3"/>
+        <v>134877.20075434781</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -2303,43 +1303,43 @@
       </c>
       <c r="F10" s="16">
         <f>F8+F9</f>
-        <v>702360</v>
+        <v>1053540</v>
       </c>
       <c r="G10" s="16">
         <f>G8+G9</f>
-        <v>799455.60000000009</v>
+        <v>1199183.4000000001</v>
       </c>
       <c r="H10" s="16">
         <f>H8+H9</f>
-        <v>823070.26800000016</v>
+        <v>1234605.402</v>
       </c>
       <c r="I10" s="16">
         <f>I8+I9</f>
-        <v>847384.15104000014</v>
+        <v>1271076.2265600003</v>
       </c>
       <c r="J10" s="16">
-        <f t="shared" ref="J10:N10" si="3">J8+J9</f>
-        <v>872417.99494620005</v>
+        <f t="shared" ref="J10:N10" si="4">J8+J9</f>
+        <v>1308626.9924193001</v>
       </c>
       <c r="K10" s="16">
-        <f t="shared" si="3"/>
-        <v>898193.16215396137</v>
+        <f t="shared" si="4"/>
+        <v>1347289.7432309417</v>
       </c>
       <c r="L10" s="16">
-        <f t="shared" si="3"/>
-        <v>924731.65006193926</v>
+        <f t="shared" si="4"/>
+        <v>1387097.4750929091</v>
       </c>
       <c r="M10" s="16">
-        <f t="shared" si="3"/>
-        <v>952056.10993324092</v>
+        <f t="shared" si="4"/>
+        <v>1428084.1648998612</v>
       </c>
       <c r="N10" s="16">
-        <f t="shared" si="3"/>
-        <v>980189.86635991756</v>
+        <f t="shared" si="4"/>
+        <v>1470284.7995398762</v>
       </c>
       <c r="O10" s="17">
         <f>O8+O9</f>
-        <v>1009156.9373076116</v>
+        <v>1513735.4059614171</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -2373,39 +1373,39 @@
         <v>0.85</v>
       </c>
       <c r="G12" s="23">
-        <f>$B$33</f>
+        <f t="shared" ref="G12:O12" si="5">$B$33</f>
         <v>0.95</v>
       </c>
       <c r="H12" s="23">
-        <f>$B$33</f>
+        <f t="shared" si="5"/>
         <v>0.95</v>
       </c>
       <c r="I12" s="23">
-        <f>$B$33</f>
+        <f t="shared" si="5"/>
         <v>0.95</v>
       </c>
       <c r="J12" s="23">
-        <f>$B$33</f>
+        <f t="shared" si="5"/>
         <v>0.95</v>
       </c>
       <c r="K12" s="23">
-        <f>$B$33</f>
+        <f t="shared" si="5"/>
         <v>0.95</v>
       </c>
       <c r="L12" s="23">
-        <f>$B$33</f>
+        <f t="shared" si="5"/>
         <v>0.95</v>
       </c>
       <c r="M12" s="23">
-        <f>$B$33</f>
+        <f t="shared" si="5"/>
         <v>0.95</v>
       </c>
       <c r="N12" s="23">
-        <f>$B$33</f>
+        <f t="shared" si="5"/>
         <v>0.95</v>
       </c>
       <c r="O12" s="24">
-        <f>$B$33</f>
+        <f t="shared" si="5"/>
         <v>0.95</v>
       </c>
     </row>
@@ -2426,43 +1426,43 @@
         <v>3000</v>
       </c>
       <c r="F13" s="26">
-        <f>E13*(1+$B$35)</f>
+        <f t="shared" ref="F13:O13" si="6">E13*(1+$B$35)</f>
         <v>3090</v>
       </c>
       <c r="G13" s="26">
-        <f>F13*(1+$B$35)</f>
+        <f t="shared" si="6"/>
         <v>3182.7000000000003</v>
       </c>
       <c r="H13" s="26">
-        <f>G13*(1+$B$35)</f>
+        <f t="shared" si="6"/>
         <v>3278.1810000000005</v>
       </c>
       <c r="I13" s="26">
-        <f>H13*(1+$B$35)</f>
+        <f t="shared" si="6"/>
         <v>3376.5264300000008</v>
       </c>
       <c r="J13" s="26">
-        <f>I13*(1+$B$35)</f>
+        <f t="shared" si="6"/>
         <v>3477.8222229000007</v>
       </c>
       <c r="K13" s="26">
-        <f>J13*(1+$B$35)</f>
+        <f t="shared" si="6"/>
         <v>3582.1568895870009</v>
       </c>
       <c r="L13" s="26">
-        <f>K13*(1+$B$35)</f>
+        <f t="shared" si="6"/>
         <v>3689.621596274611</v>
       </c>
       <c r="M13" s="26">
-        <f>L13*(1+$B$35)</f>
+        <f t="shared" si="6"/>
         <v>3800.3102441628494</v>
       </c>
       <c r="N13" s="26">
-        <f>M13*(1+$B$35)</f>
+        <f t="shared" si="6"/>
         <v>3914.3195514877348</v>
       </c>
       <c r="O13" s="27">
-        <f>N13*(1+$B$35)</f>
+        <f t="shared" si="6"/>
         <v>4031.7491380323668</v>
       </c>
     </row>
@@ -2470,8 +1470,9 @@
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="22">
-        <v>0.05</v>
+      <c r="B14" s="24">
+        <f>F23/B11</f>
+        <v>6.3339840000000008E-2</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="28" t="s">
@@ -2480,44 +1481,44 @@
       <c r="E14" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="52">
-        <f>$B$35</f>
+      <c r="F14" s="51">
+        <f t="shared" ref="F14:O14" si="7">$B$35</f>
         <v>0.03</v>
       </c>
       <c r="G14" s="30">
-        <f>$B$35</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="H14" s="30">
-        <f>$B$35</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="I14" s="30">
-        <f>$B$35</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="J14" s="30">
-        <f>$B$35</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="K14" s="30">
-        <f>$B$35</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="L14" s="30">
-        <f>$B$35</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="M14" s="30">
-        <f>$B$35</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="N14" s="30">
-        <f>$B$35</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="O14" s="31">
-        <f>$B$35</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
     </row>
@@ -2527,7 +1528,7 @@
       </c>
       <c r="B15" s="27">
         <f>B11/B7</f>
-        <v>500000</v>
+        <v>333333.33333333331</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="18"/>
@@ -2565,43 +1566,43 @@
       </c>
       <c r="F17" s="9">
         <f>$B$42*$B$7*12</f>
-        <v>288000</v>
+        <v>378000</v>
       </c>
       <c r="G17" s="9">
-        <f>F17*(1+$B$43)</f>
-        <v>295200</v>
+        <f t="shared" ref="G17:O17" si="8">F17*(1+$B$43)</f>
+        <v>387449.99999999994</v>
       </c>
       <c r="H17" s="9">
-        <f>G17*(1+$B$43)</f>
-        <v>302580</v>
+        <f t="shared" si="8"/>
+        <v>397136.24999999988</v>
       </c>
       <c r="I17" s="9">
-        <f>H17*(1+$B$43)</f>
-        <v>310144.5</v>
+        <f t="shared" si="8"/>
+        <v>407064.65624999983</v>
       </c>
       <c r="J17" s="9">
-        <f>I17*(1+$B$43)</f>
-        <v>317898.11249999999</v>
+        <f t="shared" si="8"/>
+        <v>417241.27265624981</v>
       </c>
       <c r="K17" s="9">
-        <f>J17*(1+$B$43)</f>
-        <v>325845.56531249994</v>
+        <f t="shared" si="8"/>
+        <v>427672.30447265605</v>
       </c>
       <c r="L17" s="9">
-        <f>K17*(1+$B$43)</f>
-        <v>333991.70444531238</v>
+        <f t="shared" si="8"/>
+        <v>438364.11208447244</v>
       </c>
       <c r="M17" s="9">
-        <f>L17*(1+$B$43)</f>
-        <v>342341.49705644517</v>
+        <f t="shared" si="8"/>
+        <v>449323.2148865842</v>
       </c>
       <c r="N17" s="9">
-        <f>M17*(1+$B$43)</f>
-        <v>350900.03448285628</v>
+        <f t="shared" si="8"/>
+        <v>460556.29525874875</v>
       </c>
       <c r="O17" s="10">
-        <f>N17*(1+$B$43)</f>
-        <v>359672.53534492763</v>
+        <f t="shared" si="8"/>
+        <v>472070.20264021744</v>
       </c>
     </row>
     <row r="18" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -2613,44 +1614,44 @@
         <v>35</v>
       </c>
       <c r="F18" s="9">
-        <f>F10*$B$44</f>
-        <v>28094.400000000001</v>
+        <f t="shared" ref="F18:O18" si="9">F10*$B$44</f>
+        <v>42141.599999999999</v>
       </c>
       <c r="G18" s="9">
-        <f>G10*$B$44</f>
-        <v>31978.224000000006</v>
+        <f t="shared" si="9"/>
+        <v>47967.336000000003</v>
       </c>
       <c r="H18" s="9">
-        <f>H10*$B$44</f>
-        <v>32922.810720000009</v>
+        <f t="shared" si="9"/>
+        <v>49384.216079999998</v>
       </c>
       <c r="I18" s="9">
-        <f>I10*$B$44</f>
-        <v>33895.366041600006</v>
+        <f t="shared" si="9"/>
+        <v>50843.049062400016</v>
       </c>
       <c r="J18" s="9">
-        <f>J10*$B$44</f>
-        <v>34896.719797848004</v>
+        <f t="shared" si="9"/>
+        <v>52345.079696772009</v>
       </c>
       <c r="K18" s="9">
-        <f>K10*$B$44</f>
-        <v>35927.726486158455</v>
+        <f t="shared" si="9"/>
+        <v>53891.589729237669</v>
       </c>
       <c r="L18" s="9">
-        <f>L10*$B$44</f>
-        <v>36989.266002477569</v>
+        <f t="shared" si="9"/>
+        <v>55483.89900371636</v>
       </c>
       <c r="M18" s="9">
-        <f>M10*$B$44</f>
-        <v>38082.244397329639</v>
+        <f t="shared" si="9"/>
+        <v>57123.366595994448</v>
       </c>
       <c r="N18" s="9">
-        <f>N10*$B$44</f>
-        <v>39207.5946543967</v>
+        <f t="shared" si="9"/>
+        <v>58811.39198159505</v>
       </c>
       <c r="O18" s="39">
-        <f>O10*$B$44</f>
-        <v>40366.277492304464</v>
+        <f t="shared" si="9"/>
+        <v>60549.416238456688</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -2666,43 +1667,43 @@
       </c>
       <c r="F19" s="16">
         <f>F17+F18</f>
-        <v>316094.40000000002</v>
+        <v>420141.6</v>
       </c>
       <c r="G19" s="16">
         <f>G17+G18</f>
-        <v>327178.22399999999</v>
+        <v>435417.33599999995</v>
       </c>
       <c r="H19" s="16">
         <f>H17+H18</f>
-        <v>335502.81072000001</v>
+        <v>446520.46607999987</v>
       </c>
       <c r="I19" s="16">
         <f>I17+I18</f>
-        <v>344039.86604160001</v>
+        <v>457907.70531239983</v>
       </c>
       <c r="J19" s="16">
-        <f t="shared" ref="J19:N19" si="4">J17+J18</f>
-        <v>352794.83229784801</v>
+        <f t="shared" ref="J19:N19" si="10">J17+J18</f>
+        <v>469586.35235302185</v>
       </c>
       <c r="K19" s="16">
-        <f t="shared" si="4"/>
-        <v>361773.29179865838</v>
+        <f t="shared" si="10"/>
+        <v>481563.89420189371</v>
       </c>
       <c r="L19" s="16">
-        <f t="shared" si="4"/>
-        <v>370980.97044778994</v>
+        <f t="shared" si="10"/>
+        <v>493848.0110881888</v>
       </c>
       <c r="M19" s="16">
-        <f t="shared" si="4"/>
-        <v>380423.7414537748</v>
+        <f t="shared" si="10"/>
+        <v>506446.58148257865</v>
       </c>
       <c r="N19" s="16">
-        <f t="shared" si="4"/>
-        <v>390107.62913725298</v>
+        <f t="shared" si="10"/>
+        <v>519367.68724034377</v>
       </c>
       <c r="O19" s="17">
         <f>O17+O18</f>
-        <v>400038.81283723208</v>
+        <v>532619.61887867411</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -2720,43 +1721,43 @@
       <c r="E20" s="34"/>
       <c r="F20" s="30">
         <f>IF(F10=0,0,F19/F10)</f>
-        <v>0.45004613018964634</v>
+        <v>0.39879036391594053</v>
       </c>
       <c r="G20" s="30">
         <f>IF(G10=0,0,G19/G10)</f>
-        <v>0.40925127549297291</v>
+        <v>0.36309486605635127</v>
       </c>
       <c r="H20" s="30">
         <f>IF(H10=0,0,H19/H10)</f>
-        <v>0.4076235332072522</v>
+        <v>0.36167059155634562</v>
       </c>
       <c r="I20" s="30">
         <f>IF(I10=0,0,I19/I10)</f>
-        <v>0.40600224304332055</v>
+        <v>0.36025196266290532</v>
       </c>
       <c r="J20" s="30">
-        <f t="shared" ref="J20:N20" si="5">IF(J10=0,0,J19/J10)</f>
-        <v>0.40438738579619055</v>
+        <f t="shared" ref="J20:N20" si="11">IF(J10=0,0,J19/J10)</f>
+        <v>0.35883896257166659</v>
       </c>
       <c r="K20" s="30">
-        <f t="shared" si="5"/>
-        <v>0.40277894226124822</v>
+        <f t="shared" si="11"/>
+        <v>0.3574315744785922</v>
       </c>
       <c r="L20" s="30">
-        <f t="shared" si="5"/>
-        <v>0.40117689323485506</v>
+        <f t="shared" si="11"/>
+        <v>0.35602978158049808</v>
       </c>
       <c r="M20" s="30">
-        <f t="shared" si="5"/>
-        <v>0.39958121951494063</v>
+        <f t="shared" si="11"/>
+        <v>0.35463356707557303</v>
       </c>
       <c r="N20" s="30">
-        <f t="shared" si="5"/>
-        <v>0.39799190190159411</v>
+        <f t="shared" si="11"/>
+        <v>0.35324291416389481</v>
       </c>
       <c r="O20" s="31">
         <f>IF(O10=0,0,O19/O10)</f>
-        <v>0.39640892119764731</v>
+        <v>0.35185780604794137</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -2805,43 +1806,43 @@
       </c>
       <c r="F23" s="16">
         <f>F10-F19</f>
-        <v>386265.59999999998</v>
+        <v>633398.4</v>
       </c>
       <c r="G23" s="16">
         <f>G10-G19</f>
-        <v>472277.37600000011</v>
+        <v>763766.06400000025</v>
       </c>
       <c r="H23" s="16">
         <f>H10-H19</f>
-        <v>487567.45728000015</v>
+        <v>788084.93592000008</v>
       </c>
       <c r="I23" s="16">
         <f>I10-I19</f>
-        <v>503344.28499840014</v>
+        <v>813168.52124760044</v>
       </c>
       <c r="J23" s="16">
-        <f t="shared" ref="J23:N23" si="6">J10-J19</f>
-        <v>519623.16264835204</v>
+        <f t="shared" ref="J23:N23" si="12">J10-J19</f>
+        <v>839040.64006627828</v>
       </c>
       <c r="K23" s="16">
-        <f t="shared" si="6"/>
-        <v>536419.87035530293</v>
+        <f t="shared" si="12"/>
+        <v>865725.849029048</v>
       </c>
       <c r="L23" s="16">
-        <f t="shared" si="6"/>
-        <v>553750.67961414927</v>
+        <f t="shared" si="12"/>
+        <v>893249.46400472033</v>
       </c>
       <c r="M23" s="16">
-        <f t="shared" si="6"/>
-        <v>571632.36847946607</v>
+        <f t="shared" si="12"/>
+        <v>921637.58341728256</v>
       </c>
       <c r="N23" s="16">
-        <f t="shared" si="6"/>
-        <v>590082.23722266452</v>
+        <f t="shared" si="12"/>
+        <v>950917.1122995324</v>
       </c>
       <c r="O23" s="17">
         <f>O10-O19</f>
-        <v>609118.12447037944</v>
+        <v>981115.78708274302</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -2858,43 +1859,43 @@
       </c>
       <c r="F24" s="23">
         <f>IF(F10=0,0,F23/F10)</f>
-        <v>0.54995386981035366</v>
+        <v>0.60120963608405953</v>
       </c>
       <c r="G24" s="23">
         <f>IF(G10=0,0,G23/G10)</f>
-        <v>0.59074872450702709</v>
+        <v>0.63690513394364878</v>
       </c>
       <c r="H24" s="23">
         <f>IF(H10=0,0,H23/H10)</f>
-        <v>0.5923764667927478</v>
+        <v>0.63832940844365438</v>
       </c>
       <c r="I24" s="23">
         <f>IF(I10=0,0,I23/I10)</f>
-        <v>0.59399775695667945</v>
+        <v>0.63974803733709462</v>
       </c>
       <c r="J24" s="23">
-        <f t="shared" ref="J24:N24" si="7">IF(J10=0,0,J23/J10)</f>
-        <v>0.59561261420380951</v>
+        <f t="shared" ref="J24:N24" si="13">IF(J10=0,0,J23/J10)</f>
+        <v>0.64116103742833341</v>
       </c>
       <c r="K24" s="23">
-        <f t="shared" si="7"/>
-        <v>0.59722105773875167</v>
+        <f t="shared" si="13"/>
+        <v>0.6425684255214078</v>
       </c>
       <c r="L24" s="23">
-        <f t="shared" si="7"/>
-        <v>0.59882310676514494</v>
+        <f t="shared" si="13"/>
+        <v>0.64397021841950197</v>
       </c>
       <c r="M24" s="23">
-        <f t="shared" si="7"/>
-        <v>0.60041878048505926</v>
+        <f t="shared" si="13"/>
+        <v>0.64536643292442697</v>
       </c>
       <c r="N24" s="23">
-        <f t="shared" si="7"/>
-        <v>0.60200809809840583</v>
+        <f t="shared" si="13"/>
+        <v>0.64675708583610514</v>
       </c>
       <c r="O24" s="24">
         <f>IF(O10=0,0,O23/O10)</f>
-        <v>0.60359107880235263</v>
+        <v>0.64814219395205863</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -2905,43 +1906,43 @@
       <c r="E25" s="34"/>
       <c r="F25" s="30">
         <f>F23/$B$13</f>
-        <v>3.7869176470588232E-2</v>
+        <v>6.2097882352941176E-2</v>
       </c>
       <c r="G25" s="30">
         <f>G23/$B$13</f>
-        <v>4.6301703529411778E-2</v>
+        <v>7.487902588235297E-2</v>
       </c>
       <c r="H25" s="30">
         <f>H23/$B$13</f>
-        <v>4.7800731105882364E-2</v>
+        <v>7.7263229011764717E-2</v>
       </c>
       <c r="I25" s="30">
         <f>I23/$B$13</f>
-        <v>4.934747892141178E-2</v>
+        <v>7.9722404043882394E-2</v>
       </c>
       <c r="J25" s="30">
-        <f t="shared" ref="J25:N25" si="8">J23/$B$13</f>
-        <v>5.0943447318465888E-2</v>
+        <f t="shared" ref="J25:N25" si="14">J23/$B$13</f>
+        <v>8.2258886281007679E-2</v>
       </c>
       <c r="K25" s="30">
-        <f t="shared" si="8"/>
-        <v>5.2590183368166954E-2</v>
+        <f t="shared" si="14"/>
+        <v>8.4875083238141955E-2</v>
       </c>
       <c r="L25" s="30">
-        <f t="shared" si="8"/>
-        <v>5.4289282315112673E-2</v>
+        <f t="shared" si="14"/>
+        <v>8.7573476863207877E-2</v>
       </c>
       <c r="M25" s="30">
-        <f t="shared" si="8"/>
-        <v>5.6042389066614323E-2</v>
+        <f t="shared" si="14"/>
+        <v>9.0356625825223774E-2</v>
       </c>
       <c r="N25" s="30">
-        <f t="shared" si="8"/>
-        <v>5.7851199727712209E-2</v>
+        <f t="shared" si="14"/>
+        <v>9.322716787250318E-2</v>
       </c>
       <c r="O25" s="31">
         <f>O23/$B$13</f>
-        <v>5.9717463183370532E-2</v>
+        <v>9.6187822263014019E-2</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -2958,7 +1959,7 @@
       </c>
       <c r="B27" s="22">
         <f>B14</f>
-        <v>0.05</v>
+        <v>6.3339840000000008E-2</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="2" t="s">
@@ -2989,43 +1990,43 @@
       <c r="E28" s="34"/>
       <c r="F28" s="38">
         <f>$B$46*$B$7</f>
-        <v>36000</v>
+        <v>54000</v>
       </c>
       <c r="G28" s="38">
-        <f>F28*(1+$B$47)</f>
-        <v>36720</v>
+        <f t="shared" ref="G28:O28" si="15">F28*(1+$B$47)</f>
+        <v>55080</v>
       </c>
       <c r="H28" s="38">
-        <f>G28*(1+$B$47)</f>
-        <v>37454.400000000001</v>
+        <f t="shared" si="15"/>
+        <v>56181.599999999999</v>
       </c>
       <c r="I28" s="38">
-        <f>H28*(1+$B$47)</f>
-        <v>38203.488000000005</v>
+        <f t="shared" si="15"/>
+        <v>57305.231999999996</v>
       </c>
       <c r="J28" s="38">
-        <f>I28*(1+$B$47)</f>
-        <v>38967.557760000003</v>
+        <f t="shared" si="15"/>
+        <v>58451.336639999994</v>
       </c>
       <c r="K28" s="38">
-        <f>J28*(1+$B$47)</f>
-        <v>39746.908915200002</v>
+        <f t="shared" si="15"/>
+        <v>59620.363372799999</v>
       </c>
       <c r="L28" s="38">
-        <f>K28*(1+$B$47)</f>
-        <v>40541.847093504002</v>
+        <f t="shared" si="15"/>
+        <v>60812.770640256</v>
       </c>
       <c r="M28" s="38">
-        <f>L28*(1+$B$47)</f>
-        <v>41352.684035374084</v>
+        <f t="shared" si="15"/>
+        <v>62029.026053061119</v>
       </c>
       <c r="N28" s="38">
-        <f>M28*(1+$B$47)</f>
-        <v>42179.737716081567</v>
+        <f t="shared" si="15"/>
+        <v>63269.606574122343</v>
       </c>
       <c r="O28" s="39">
-        <f>N28*(1+$B$47)</f>
-        <v>43023.332470403198</v>
+        <f t="shared" si="15"/>
+        <v>64534.99870560479</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -3033,7 +2034,7 @@
         <v>54</v>
       </c>
       <c r="B29" s="14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C29" s="33"/>
       <c r="D29" s="18"/>
@@ -3066,43 +2067,43 @@
         <v>55</v>
       </c>
       <c r="F31" s="26">
-        <f>IF(COLUMN()-COLUMN($E$31)&gt;$B$29,"-",F35*$B$21)</f>
+        <f t="shared" ref="F31:O31" si="16">IF(COLUMN()-COLUMN($E$31)&gt;$B$29,"-",F35*$B$21)</f>
         <v>357500</v>
       </c>
       <c r="G31" s="26">
-        <f>IF(COLUMN()-COLUMN($E$31)&gt;$B$29,"-",G35*$B$21)</f>
+        <f t="shared" si="16"/>
         <v>357500</v>
       </c>
       <c r="H31" s="26">
-        <f>IF(COLUMN()-COLUMN($E$31)&gt;$B$29,"-",H35*$B$21)</f>
+        <f t="shared" si="16"/>
         <v>357500</v>
       </c>
       <c r="I31" s="26">
-        <f>IF(COLUMN()-COLUMN($E$31)&gt;$B$29,"-",I35*$B$21)</f>
+        <f t="shared" si="16"/>
         <v>351832.32544979226</v>
       </c>
       <c r="J31" s="26">
-        <f>IF(COLUMN()-COLUMN($E$31)&gt;$B$29,"-",J35*$B$21)</f>
+        <f t="shared" si="16"/>
         <v>345844.94950484572</v>
       </c>
-      <c r="K31" s="26" t="str">
-        <f>IF(COLUMN()-COLUMN($E$31)&gt;$B$29,"-",K35*$B$21)</f>
+      <c r="K31" s="26">
+        <f t="shared" si="16"/>
+        <v>339519.83849352098</v>
+      </c>
+      <c r="L31" s="26">
+        <f t="shared" si="16"/>
+        <v>332837.94150334637</v>
+      </c>
+      <c r="M31" s="26" t="str">
+        <f t="shared" si="16"/>
         <v>-</v>
       </c>
-      <c r="L31" s="26" t="str">
-        <f>IF(COLUMN()-COLUMN($E$31)&gt;$B$29,"-",L35*$B$21)</f>
+      <c r="N31" s="26" t="str">
+        <f t="shared" si="16"/>
         <v>-</v>
       </c>
-      <c r="M31" s="26" t="str">
-        <f>IF(COLUMN()-COLUMN($E$31)&gt;$B$29,"-",M35*$B$21)</f>
-        <v>-</v>
-      </c>
-      <c r="N31" s="26" t="str">
-        <f>IF(COLUMN()-COLUMN($E$31)&gt;$B$29,"-",N35*$B$21)</f>
-        <v>-</v>
-      </c>
       <c r="O31" s="27" t="str">
-        <f>IF(COLUMN()-COLUMN($E$31)&gt;$B$29,"-",O35*$B$21)</f>
+        <f t="shared" si="16"/>
         <v>-</v>
       </c>
     </row>
@@ -3117,43 +2118,43 @@
         <v>56</v>
       </c>
       <c r="F32" s="26">
-        <f>IF(COLUMN()-COLUMN($E$32)&gt;$B$29,"-",IF(COLUMN(F32)-COLUMN($F$32)+1&lt;=$B$23, 0, -PPMT($B$21/12, (COLUMN(F32)-COLUMN($F$32)+1-$B$23)*12, ($B$22-$B$23)*12, $B$20)*12))</f>
+        <f t="shared" ref="F32:O32" si="17">IF(COLUMN()-COLUMN($E$32)&gt;$B$29,"-",IF(COLUMN(F32)-COLUMN($F$32)+1&lt;=$B$23, 0, -PPMT($B$21/12, (COLUMN(F32)-COLUMN($F$32)+1-$B$23)*12, ($B$22-$B$23)*12, $B$20)*12))</f>
         <v>0</v>
       </c>
       <c r="G32" s="26">
-        <f>IF(COLUMN()-COLUMN($E$32)&gt;$B$29,"-",IF(COLUMN(G32)-COLUMN($F$32)+1&lt;=$B$23, 0, -PPMT($B$21/12, (COLUMN(G32)-COLUMN($F$32)+1-$B$23)*12, ($B$22-$B$23)*12, $B$20)*12))</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="H32" s="26">
-        <f>IF(COLUMN()-COLUMN($E$32)&gt;$B$29,"-",IF(COLUMN(H32)-COLUMN($F$32)+1&lt;=$B$23, 0, -PPMT($B$21/12, (COLUMN(H32)-COLUMN($F$32)+1-$B$23)*12, ($B$22-$B$23)*12, $B$20)*12))</f>
+        <f t="shared" si="17"/>
         <v>103048.62818559544</v>
       </c>
       <c r="I32" s="26">
-        <f>IF(COLUMN()-COLUMN($E$32)&gt;$B$29,"-",IF(COLUMN(I32)-COLUMN($F$32)+1&lt;=$B$23, 0, -PPMT($B$21/12, (COLUMN(I32)-COLUMN($F$32)+1-$B$23)*12, ($B$22-$B$23)*12, $B$20)*12))</f>
+        <f t="shared" si="17"/>
         <v>108861.38081720944</v>
       </c>
       <c r="J32" s="26">
-        <f>IF(COLUMN()-COLUMN($E$32)&gt;$B$29,"-",IF(COLUMN(J32)-COLUMN($F$32)+1&lt;=$B$23, 0, -PPMT($B$21/12, (COLUMN(J32)-COLUMN($F$32)+1-$B$23)*12, ($B$22-$B$23)*12, $B$20)*12))</f>
+        <f t="shared" si="17"/>
         <v>115002.01838772319</v>
       </c>
-      <c r="K32" s="26" t="str">
-        <f>IF(COLUMN()-COLUMN($E$32)&gt;$B$29,"-",IF(COLUMN(K32)-COLUMN($F$32)+1&lt;=$B$23, 0, -PPMT($B$21/12, (COLUMN(K32)-COLUMN($F$32)+1-$B$23)*12, ($B$22-$B$23)*12, $B$20)*12))</f>
+      <c r="K32" s="26">
+        <f t="shared" si="17"/>
+        <v>121489.03618499266</v>
+      </c>
+      <c r="L32" s="26">
+        <f t="shared" si="17"/>
+        <v>128341.97277648898</v>
+      </c>
+      <c r="M32" s="26" t="str">
+        <f t="shared" si="17"/>
         <v>-</v>
       </c>
-      <c r="L32" s="26" t="str">
-        <f>IF(COLUMN()-COLUMN($E$32)&gt;$B$29,"-",IF(COLUMN(L32)-COLUMN($F$32)+1&lt;=$B$23, 0, -PPMT($B$21/12, (COLUMN(L32)-COLUMN($F$32)+1-$B$23)*12, ($B$22-$B$23)*12, $B$20)*12))</f>
+      <c r="N32" s="26" t="str">
+        <f t="shared" si="17"/>
         <v>-</v>
       </c>
-      <c r="M32" s="26" t="str">
-        <f>IF(COLUMN()-COLUMN($E$32)&gt;$B$29,"-",IF(COLUMN(M32)-COLUMN($F$32)+1&lt;=$B$23, 0, -PPMT($B$21/12, (COLUMN(M32)-COLUMN($F$32)+1-$B$23)*12, ($B$22-$B$23)*12, $B$20)*12))</f>
-        <v>-</v>
-      </c>
-      <c r="N32" s="26" t="str">
-        <f>IF(COLUMN()-COLUMN($E$32)&gt;$B$29,"-",IF(COLUMN(N32)-COLUMN($F$32)+1&lt;=$B$23, 0, -PPMT($B$21/12, (COLUMN(N32)-COLUMN($F$32)+1-$B$23)*12, ($B$22-$B$23)*12, $B$20)*12))</f>
-        <v>-</v>
-      </c>
       <c r="O32" s="27" t="str">
-        <f>IF(COLUMN()-COLUMN($E$32)&gt;$B$29,"-",IF(COLUMN(O32)-COLUMN($F$32)+1&lt;=$B$23, 0, -PPMT($B$21/12, (COLUMN(O32)-COLUMN($F$32)+1-$B$23)*12, ($B$22-$B$23)*12, $B$20)*12))</f>
+        <f t="shared" si="17"/>
         <v>-</v>
       </c>
     </row>
@@ -3167,44 +2168,44 @@
       <c r="D33" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="57">
-        <f>IF(COLUMN()-COLUMN($E$33)&gt;$B$29,"-",F31+F32)</f>
+      <c r="F33" s="54">
+        <f t="shared" ref="F33:O33" si="18">IF(COLUMN()-COLUMN($E$33)&gt;$B$29,"-",F31+F32)</f>
         <v>357500</v>
       </c>
-      <c r="G33" s="57">
-        <f>IF(COLUMN()-COLUMN($E$33)&gt;$B$29,"-",G31+G32)</f>
+      <c r="G33" s="54">
+        <f t="shared" si="18"/>
         <v>357500</v>
       </c>
-      <c r="H33" s="57">
-        <f>IF(COLUMN()-COLUMN($E$33)&gt;$B$29,"-",H31+H32)</f>
+      <c r="H33" s="54">
+        <f t="shared" si="18"/>
         <v>460548.62818559544</v>
       </c>
-      <c r="I33" s="57">
-        <f>IF(COLUMN()-COLUMN($E$33)&gt;$B$29,"-",I31+I32)</f>
+      <c r="I33" s="54">
+        <f t="shared" si="18"/>
         <v>460693.70626700169</v>
       </c>
-      <c r="J33" s="57">
-        <f>IF(COLUMN()-COLUMN($E$33)&gt;$B$29,"-",J31+J32)</f>
+      <c r="J33" s="54">
+        <f t="shared" si="18"/>
         <v>460846.96789256891</v>
       </c>
-      <c r="K33" s="57" t="str">
-        <f>IF(COLUMN()-COLUMN($E$33)&gt;$B$29,"-",K31+K32)</f>
+      <c r="K33" s="54">
+        <f t="shared" si="18"/>
+        <v>461008.87467851362</v>
+      </c>
+      <c r="L33" s="54">
+        <f t="shared" si="18"/>
+        <v>461179.91427983536</v>
+      </c>
+      <c r="M33" s="54" t="str">
+        <f t="shared" si="18"/>
         <v>-</v>
       </c>
-      <c r="L33" s="57" t="str">
-        <f>IF(COLUMN()-COLUMN($E$33)&gt;$B$29,"-",L31+L32)</f>
+      <c r="N33" s="54" t="str">
+        <f t="shared" si="18"/>
         <v>-</v>
       </c>
-      <c r="M33" s="57" t="str">
-        <f>IF(COLUMN()-COLUMN($E$33)&gt;$B$29,"-",M31+M32)</f>
-        <v>-</v>
-      </c>
-      <c r="N33" s="57" t="str">
-        <f>IF(COLUMN()-COLUMN($E$33)&gt;$B$29,"-",N31+N32)</f>
-        <v>-</v>
-      </c>
       <c r="O33" s="36" t="str">
-        <f>IF(COLUMN()-COLUMN($E$33)&gt;$B$29,"-",O31+O32)</f>
+        <f t="shared" si="18"/>
         <v>-</v>
       </c>
     </row>
@@ -3221,43 +2222,43 @@
       </c>
       <c r="E34" s="34"/>
       <c r="F34" s="40">
-        <f>IF(COLUMN()-COLUMN($E$34)&gt;$B$29,"-",IF(F33=0,0,F23/F33))</f>
-        <v>1.0804632167832167</v>
+        <f t="shared" ref="F34:O34" si="19">IF(COLUMN()-COLUMN($E$34)&gt;$B$29,"-",IF(F33=0,0,F23/F33))</f>
+        <v>1.7717437762237762</v>
       </c>
       <c r="G34" s="40">
-        <f>IF(COLUMN()-COLUMN($E$34)&gt;$B$29,"-",IF(G33=0,0,G23/G33))</f>
-        <v>1.3210555972027975</v>
+        <f t="shared" si="19"/>
+        <v>2.1364085706293712</v>
       </c>
       <c r="H34" s="40">
-        <f>IF(COLUMN()-COLUMN($E$34)&gt;$B$29,"-",IF(H33=0,0,H23/H33))</f>
-        <v>1.0586666150778685</v>
+        <f t="shared" si="19"/>
+        <v>1.7111872399333508</v>
       </c>
       <c r="I34" s="40">
-        <f>IF(COLUMN()-COLUMN($E$34)&gt;$B$29,"-",IF(I33=0,0,I23/I33))</f>
-        <v>1.092579034944922</v>
+        <f t="shared" si="19"/>
+        <v>1.7650957896444908</v>
       </c>
       <c r="J34" s="40">
-        <f>IF(COLUMN()-COLUMN($E$34)&gt;$B$29,"-",IF(J33=0,0,J23/J33))</f>
-        <v>1.1275395062802818</v>
-      </c>
-      <c r="K34" s="40" t="str">
-        <f>IF(COLUMN()-COLUMN($E$34)&gt;$B$29,"-",IF(K33=0,0,K23/K33))</f>
+        <f t="shared" si="19"/>
+        <v>1.8206491493329573</v>
+      </c>
+      <c r="K34" s="40">
+        <f t="shared" si="19"/>
+        <v>1.8778941069903814</v>
+      </c>
+      <c r="L34" s="40">
+        <f t="shared" si="19"/>
+        <v>1.9368785073816404</v>
+      </c>
+      <c r="M34" s="40" t="str">
+        <f t="shared" si="19"/>
         <v>-</v>
       </c>
-      <c r="L34" s="40" t="str">
-        <f>IF(COLUMN()-COLUMN($E$34)&gt;$B$29,"-",IF(L33=0,0,L23/L33))</f>
+      <c r="N34" s="40" t="str">
+        <f t="shared" si="19"/>
         <v>-</v>
       </c>
-      <c r="M34" s="40" t="str">
-        <f>IF(COLUMN()-COLUMN($E$34)&gt;$B$29,"-",IF(M33=0,0,M23/M33))</f>
-        <v>-</v>
-      </c>
-      <c r="N34" s="40" t="str">
-        <f>IF(COLUMN()-COLUMN($E$34)&gt;$B$29,"-",IF(N33=0,0,N23/N33))</f>
-        <v>-</v>
-      </c>
       <c r="O34" s="41" t="str">
-        <f>IF(COLUMN()-COLUMN($E$34)&gt;$B$29,"-",IF(O33=0,0,O23/O33))</f>
+        <f t="shared" si="19"/>
         <v>-</v>
       </c>
     </row>
@@ -3272,47 +2273,47 @@
       <c r="D35" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E35" s="58" t="s">
+      <c r="E35" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="60">
+      <c r="F35" s="57">
         <f>IF(COLUMN()-COLUMN($E$35)&gt;$B$29,"-",$B$20)</f>
         <v>6500000</v>
       </c>
-      <c r="G35" s="60">
-        <f>IF(COLUMN()-COLUMN($E$35)&gt;$B$29,"-",F36)</f>
+      <c r="G35" s="57">
+        <f t="shared" ref="G35:O35" si="20">IF(COLUMN()-COLUMN($E$35)&gt;$B$29,"-",F36)</f>
         <v>6500000</v>
       </c>
-      <c r="H35" s="60">
-        <f>IF(COLUMN()-COLUMN($E$35)&gt;$B$29,"-",G36)</f>
+      <c r="H35" s="57">
+        <f t="shared" si="20"/>
         <v>6500000</v>
       </c>
-      <c r="I35" s="60">
-        <f>IF(COLUMN()-COLUMN($E$35)&gt;$B$29,"-",H36)</f>
+      <c r="I35" s="57">
+        <f t="shared" si="20"/>
         <v>6396951.3718144046</v>
       </c>
-      <c r="J35" s="60">
-        <f>IF(COLUMN()-COLUMN($E$35)&gt;$B$29,"-",I36)</f>
+      <c r="J35" s="57">
+        <f t="shared" si="20"/>
         <v>6288089.9909971952</v>
       </c>
-      <c r="K35" s="60" t="str">
-        <f>IF(COLUMN()-COLUMN($E$35)&gt;$B$29,"-",J36)</f>
+      <c r="K35" s="57">
+        <f t="shared" si="20"/>
+        <v>6173087.9726094725</v>
+      </c>
+      <c r="L35" s="57">
+        <f t="shared" si="20"/>
+        <v>6051598.9364244798</v>
+      </c>
+      <c r="M35" s="57" t="str">
+        <f t="shared" si="20"/>
         <v>-</v>
       </c>
-      <c r="L35" s="60" t="str">
-        <f>IF(COLUMN()-COLUMN($E$35)&gt;$B$29,"-",K36)</f>
+      <c r="N35" s="57" t="str">
+        <f t="shared" si="20"/>
         <v>-</v>
       </c>
-      <c r="M35" s="60" t="str">
-        <f>IF(COLUMN()-COLUMN($E$35)&gt;$B$29,"-",L36)</f>
-        <v>-</v>
-      </c>
-      <c r="N35" s="60" t="str">
-        <f>IF(COLUMN()-COLUMN($E$35)&gt;$B$29,"-",M36)</f>
-        <v>-</v>
-      </c>
-      <c r="O35" s="61" t="str">
-        <f>IF(COLUMN()-COLUMN($E$35)&gt;$B$29,"-",N36)</f>
+      <c r="O35" s="58" t="str">
+        <f t="shared" si="20"/>
         <v>-</v>
       </c>
     </row>
@@ -3327,47 +2328,47 @@
       <c r="D36" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E36" s="59" t="s">
+      <c r="E36" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="62">
-        <f>IF(COLUMN()-COLUMN($E$36)&gt;$B$29,"-",F35-F32)</f>
+      <c r="F36" s="59">
+        <f t="shared" ref="F36:O36" si="21">IF(COLUMN()-COLUMN($E$36)&gt;$B$29,"-",F35-F32)</f>
         <v>6500000</v>
       </c>
-      <c r="G36" s="62">
-        <f>IF(COLUMN()-COLUMN($E$36)&gt;$B$29,"-",G35-G32)</f>
+      <c r="G36" s="59">
+        <f t="shared" si="21"/>
         <v>6500000</v>
       </c>
-      <c r="H36" s="62">
-        <f>IF(COLUMN()-COLUMN($E$36)&gt;$B$29,"-",H35-H32)</f>
+      <c r="H36" s="59">
+        <f t="shared" si="21"/>
         <v>6396951.3718144046</v>
       </c>
-      <c r="I36" s="62">
-        <f>IF(COLUMN()-COLUMN($E$36)&gt;$B$29,"-",I35-I32)</f>
+      <c r="I36" s="59">
+        <f t="shared" si="21"/>
         <v>6288089.9909971952</v>
       </c>
-      <c r="J36" s="62">
-        <f>IF(COLUMN()-COLUMN($E$36)&gt;$B$29,"-",J35-J32)</f>
+      <c r="J36" s="59">
+        <f t="shared" si="21"/>
         <v>6173087.9726094725</v>
       </c>
-      <c r="K36" s="62" t="str">
-        <f>IF(COLUMN()-COLUMN($E$36)&gt;$B$29,"-",K35-K32)</f>
+      <c r="K36" s="59">
+        <f t="shared" si="21"/>
+        <v>6051598.9364244798</v>
+      </c>
+      <c r="L36" s="59">
+        <f t="shared" si="21"/>
+        <v>5923256.9636479905</v>
+      </c>
+      <c r="M36" s="59" t="str">
+        <f t="shared" si="21"/>
         <v>-</v>
       </c>
-      <c r="L36" s="62" t="str">
-        <f>IF(COLUMN()-COLUMN($E$36)&gt;$B$29,"-",L35-L32)</f>
+      <c r="N36" s="59" t="str">
+        <f t="shared" si="21"/>
         <v>-</v>
       </c>
-      <c r="M36" s="62" t="str">
-        <f>IF(COLUMN()-COLUMN($E$36)&gt;$B$29,"-",M35-M32)</f>
-        <v>-</v>
-      </c>
-      <c r="N36" s="62" t="str">
-        <f>IF(COLUMN()-COLUMN($E$36)&gt;$B$29,"-",N35-N32)</f>
-        <v>-</v>
-      </c>
-      <c r="O36" s="63" t="str">
-        <f>IF(COLUMN()-COLUMN($E$36)&gt;$B$29,"-",O35-O32)</f>
+      <c r="O36" s="60" t="str">
+        <f t="shared" si="21"/>
         <v>-</v>
       </c>
     </row>
@@ -3405,45 +2406,45 @@
       <c r="O38" s="3"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="53"/>
-      <c r="B39" s="54"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="33"/>
       <c r="D39" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="66">
+      <c r="E39" s="68">
         <f>-$B$13</f>
         <v>-10200000</v>
       </c>
-      <c r="F39" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="G39" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="H39" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="I39" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="J39" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="K39" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="L39" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="M39" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="N39" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="O39" s="68" t="s">
-        <v>29</v>
+      <c r="F39" s="68">
+        <v>0</v>
+      </c>
+      <c r="G39" s="68">
+        <v>0</v>
+      </c>
+      <c r="H39" s="68">
+        <v>0</v>
+      </c>
+      <c r="I39" s="68">
+        <v>0</v>
+      </c>
+      <c r="J39" s="68">
+        <v>0</v>
+      </c>
+      <c r="K39" s="68">
+        <v>0</v>
+      </c>
+      <c r="L39" s="68">
+        <v>0</v>
+      </c>
+      <c r="M39" s="68">
+        <v>0</v>
+      </c>
+      <c r="N39" s="68">
+        <v>0</v>
+      </c>
+      <c r="O39" s="71">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -3454,94 +2455,94 @@
       <c r="D40" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="E40" ca="1">IF(COLUMN()-COLUMN($E$40)=$B$29, (INDIRECT(ADDRESS(ROW()-17,COLUMN()))*(1+$B$35))/$B$27*(1-$B$28), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="F40" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="F40" ca="1">IF(COLUMN()-COLUMN($E$40)=$B$29, (INDIRECT(ADDRESS(ROW()-17,COLUMN()))*(1+$B$35))/$B$27*(1-$B$28), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="G40" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="G40" ca="1">IF(COLUMN()-COLUMN($E$40)=$B$29, (INDIRECT(ADDRESS(ROW()-17,COLUMN()))*(1+$B$35))/$B$27*(1-$B$28), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="H40" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="H40" ca="1">IF(COLUMN()-COLUMN($E$40)=$B$29, (INDIRECT(ADDRESS(ROW()-17,COLUMN()))*(1+$B$35))/$B$27*(1-$B$28), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="I40" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="I40" ca="1">IF(COLUMN()-COLUMN($E$40)=$B$29, (INDIRECT(ADDRESS(ROW()-17,COLUMN()))*(1+$B$35))/$B$27*(1-$B$28), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="J40" s="67" cm="1">
-        <f t="array" aca="1" ref="J40" ca="1">IF(COLUMN()-COLUMN($E$40)=$B$29, (INDIRECT(ADDRESS(ROW()-17,COLUMN()))*(1+$B$35))/$B$27*(1-$B$28), "-")</f>
-        <v>10490152.40754493</v>
-      </c>
-      <c r="K40" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="K40" ca="1">IF(COLUMN()-COLUMN($E$40)=$B$29, (INDIRECT(ADDRESS(ROW()-17,COLUMN()))*(1+$B$35))/$B$27*(1-$B$28), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="L40" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="L40" ca="1">IF(COLUMN()-COLUMN($E$40)=$B$29, (INDIRECT(ADDRESS(ROW()-17,COLUMN()))*(1+$B$35))/$B$27*(1-$B$28), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="M40" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="M40" ca="1">IF(COLUMN()-COLUMN($E$40)=$B$29, (INDIRECT(ADDRESS(ROW()-17,COLUMN()))*(1+$B$35))/$B$27*(1-$B$28), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="N40" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="N40" ca="1">IF(COLUMN()-COLUMN($E$40)=$B$29, (INDIRECT(ADDRESS(ROW()-17,COLUMN()))*(1+$B$35))/$B$27*(1-$B$28), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="O40" s="69" t="str" cm="1">
-        <f t="array" aca="1" ref="O40" ca="1">IF(COLUMN()-COLUMN($E$40)=$B$29, (INDIRECT(ADDRESS(ROW()-17,COLUMN()))*(1+$B$35))/$B$27*(1-$B$28), "-")</f>
-        <v>-</v>
+      <c r="E40" s="68">
+        <f>IF(COLUMN()-COLUMN($E$40)=$B$29, (E23*(1+$B$35))/$B$27*(1-$B$28), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="68">
+        <f t="shared" ref="F40:O40" si="22">IF(COLUMN()-COLUMN($E$40)=$B$29, (F23*(1+$B$35))/$B$27*(1-$B$28), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="68">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="68">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="68">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="68">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="68">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="L40" s="68">
+        <f t="shared" si="22"/>
+        <v>14235053.466607504</v>
+      </c>
+      <c r="M40" s="68">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N40" s="68">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="O40" s="71">
+        <f t="shared" si="22"/>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="51" t="s">
+      <c r="A41" s="18" t="s">
         <v>84</v>
       </c>
       <c r="B41" s="22">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E41" s="66">
+      <c r="E41" s="68">
         <f>$B$20</f>
         <v>6500000</v>
       </c>
-      <c r="F41" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="G41" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="H41" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="I41" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="J41" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="K41" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="L41" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="M41" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="N41" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="O41" s="68" t="s">
-        <v>29</v>
+      <c r="F41" s="68">
+        <v>0</v>
+      </c>
+      <c r="G41" s="68">
+        <v>0</v>
+      </c>
+      <c r="H41" s="68">
+        <v>0</v>
+      </c>
+      <c r="I41" s="68">
+        <v>0</v>
+      </c>
+      <c r="J41" s="68">
+        <v>0</v>
+      </c>
+      <c r="K41" s="68">
+        <v>0</v>
+      </c>
+      <c r="L41" s="68">
+        <v>0</v>
+      </c>
+      <c r="M41" s="68">
+        <v>0</v>
+      </c>
+      <c r="N41" s="68">
+        <v>0</v>
+      </c>
+      <c r="O41" s="71">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -3550,54 +2551,54 @@
       </c>
       <c r="B42" s="19">
         <f>B41*B34</f>
-        <v>1200</v>
+        <v>1050</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E42" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="E42" ca="1">IF(COLUMN()-COLUMN($E$42)=$B$29, -INDIRECT(ADDRESS(ROW()-6,COLUMN())), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="F42" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="F42" ca="1">IF(COLUMN()-COLUMN($E$42)=$B$29, -INDIRECT(ADDRESS(ROW()-6,COLUMN())), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="G42" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="G42" ca="1">IF(COLUMN()-COLUMN($E$42)=$B$29, -INDIRECT(ADDRESS(ROW()-6,COLUMN())), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="H42" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="H42" ca="1">IF(COLUMN()-COLUMN($E$42)=$B$29, -INDIRECT(ADDRESS(ROW()-6,COLUMN())), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="I42" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="I42" ca="1">IF(COLUMN()-COLUMN($E$42)=$B$29, -INDIRECT(ADDRESS(ROW()-6,COLUMN())), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="J42" s="67" cm="1">
-        <f t="array" aca="1" ref="J42" ca="1">IF(COLUMN()-COLUMN($E$42)=$B$29, -INDIRECT(ADDRESS(ROW()-6,COLUMN())), "-")</f>
-        <v>-6173087.9726094725</v>
-      </c>
-      <c r="K42" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="K42" ca="1">IF(COLUMN()-COLUMN($E$42)=$B$29, -INDIRECT(ADDRESS(ROW()-6,COLUMN())), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="L42" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="L42" ca="1">IF(COLUMN()-COLUMN($E$42)=$B$29, -INDIRECT(ADDRESS(ROW()-6,COLUMN())), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="M42" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="M42" ca="1">IF(COLUMN()-COLUMN($E$42)=$B$29, -INDIRECT(ADDRESS(ROW()-6,COLUMN())), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="N42" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="N42" ca="1">IF(COLUMN()-COLUMN($E$42)=$B$29, -INDIRECT(ADDRESS(ROW()-6,COLUMN())), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="O42" s="68" t="str" cm="1">
-        <f t="array" aca="1" ref="O42" ca="1">IF(COLUMN()-COLUMN($E$42)=$B$29, -INDIRECT(ADDRESS(ROW()-6,COLUMN())), "-")</f>
-        <v>-</v>
+      <c r="E42" s="72">
+        <f>IF(COLUMN()-COLUMN($E$42)=$B$29, -E36, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="72">
+        <f t="shared" ref="F42:O42" si="23">IF(COLUMN()-COLUMN($E$42)=$B$29, -F36, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="72">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="H42" s="72">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="72">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="72">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="72">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="L42" s="72">
+        <f t="shared" si="23"/>
+        <v>-5923256.9636479905</v>
+      </c>
+      <c r="M42" s="72">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="N42" s="72">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="O42" s="71">
+        <f t="shared" si="23"/>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -3608,17 +2609,17 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D43" s="5"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="70"/>
-      <c r="H43" s="70"/>
-      <c r="I43" s="70"/>
-      <c r="J43" s="70"/>
-      <c r="K43" s="70"/>
-      <c r="L43" s="70"/>
-      <c r="M43" s="70"/>
-      <c r="N43" s="70"/>
-      <c r="O43" s="71"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="69"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="69"/>
+      <c r="I43" s="69"/>
+      <c r="J43" s="69"/>
+      <c r="K43" s="69"/>
+      <c r="L43" s="69"/>
+      <c r="M43" s="69"/>
+      <c r="N43" s="69"/>
+      <c r="O43" s="70"/>
     </row>
     <row r="44" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
@@ -3637,43 +2638,43 @@
       </c>
       <c r="F44" s="43">
         <f>F23-F28+IF(COLUMN()-COLUMN($E$44)=$B$29,F40,0)</f>
-        <v>350265.59999999998</v>
+        <v>579398.40000000002</v>
       </c>
       <c r="G44" s="43">
-        <f t="shared" ref="G44:O44" si="9">G23-G28+IF(COLUMN()-COLUMN($E$44)=$B$29,G40,0)</f>
-        <v>435557.37600000011</v>
+        <f t="shared" ref="G44:O44" si="24">G23-G28+IF(COLUMN()-COLUMN($E$44)=$B$29,G40,0)</f>
+        <v>708686.06400000025</v>
       </c>
       <c r="H44" s="43">
-        <f t="shared" si="9"/>
-        <v>450113.05728000012</v>
+        <f t="shared" si="24"/>
+        <v>731903.3359200001</v>
       </c>
       <c r="I44" s="43">
-        <f t="shared" si="9"/>
-        <v>465140.79699840012</v>
+        <f t="shared" si="24"/>
+        <v>755863.28924760048</v>
       </c>
       <c r="J44" s="43">
-        <f t="shared" ca="1" si="9"/>
-        <v>10970808.012433281</v>
+        <f t="shared" si="24"/>
+        <v>780589.30342627829</v>
       </c>
       <c r="K44" s="43">
-        <f t="shared" si="9"/>
-        <v>496672.96144010295</v>
+        <f t="shared" si="24"/>
+        <v>806105.48565624794</v>
       </c>
       <c r="L44" s="43">
-        <f t="shared" si="9"/>
-        <v>513208.83252064529</v>
+        <f t="shared" si="24"/>
+        <v>15067490.159971967</v>
       </c>
       <c r="M44" s="43">
-        <f t="shared" si="9"/>
-        <v>530279.68444409198</v>
+        <f t="shared" si="24"/>
+        <v>859608.55736422143</v>
       </c>
       <c r="N44" s="43">
-        <f t="shared" si="9"/>
-        <v>547902.49950658297</v>
-      </c>
-      <c r="O44" s="75">
-        <f t="shared" si="9"/>
-        <v>566094.79199997627</v>
+        <f t="shared" si="24"/>
+        <v>887647.50572541007</v>
+      </c>
+      <c r="O44" s="66">
+        <f t="shared" si="24"/>
+        <v>916580.7883771382</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3692,43 +2693,43 @@
         <v>-3700000</v>
       </c>
       <c r="F45" s="44">
-        <f>IF(COLUMN()-COLUMN($E$45)&gt;$B$29,"-",F23-F28-F33+IF(COLUMN()-COLUMN($E$45)=$B$29,F40+F42,0))</f>
-        <v>-7234.4000000000233</v>
+        <f t="shared" ref="F45:O45" si="25">IF(COLUMN()-COLUMN($E$45)&gt;$B$29,"-",F23-F28-F33+IF(COLUMN()-COLUMN($E$45)=$B$29,F40+F42,0))</f>
+        <v>221898.40000000002</v>
       </c>
       <c r="G45" s="44">
-        <f>IF(COLUMN()-COLUMN($E$45)&gt;$B$29,"-",G23-G28-G33+IF(COLUMN()-COLUMN($E$45)=$B$29,G40+G42,0))</f>
-        <v>78057.376000000106</v>
+        <f t="shared" si="25"/>
+        <v>351186.06400000025</v>
       </c>
       <c r="H45" s="44">
-        <f>IF(COLUMN()-COLUMN($E$45)&gt;$B$29,"-",H23-H28-H33+IF(COLUMN()-COLUMN($E$45)=$B$29,H40+H42,0))</f>
-        <v>-10435.570905595319</v>
+        <f t="shared" si="25"/>
+        <v>271354.70773440466</v>
       </c>
       <c r="I45" s="44">
-        <f>IF(COLUMN()-COLUMN($E$45)&gt;$B$29,"-",I23-I28-I33+IF(COLUMN()-COLUMN($E$45)=$B$29,I40+I42,0))</f>
-        <v>4447.0907313984353</v>
+        <f t="shared" si="25"/>
+        <v>295169.58298059879</v>
       </c>
       <c r="J45" s="44">
-        <f ca="1">IF(COLUMN()-COLUMN($E$45)&gt;$B$29,"-",J23-J28-J33+IF(COLUMN()-COLUMN($E$45)=$B$29,J40+J42,0))</f>
-        <v>4336873.0719312401</v>
-      </c>
-      <c r="K45" s="44" t="str">
-        <f>IF(COLUMN()-COLUMN($E$45)&gt;$B$29,"-",K23-K28-K33+IF(COLUMN()-COLUMN($E$45)=$B$29,K40+K42,0))</f>
+        <f t="shared" si="25"/>
+        <v>319742.33553370938</v>
+      </c>
+      <c r="K45" s="44">
+        <f t="shared" si="25"/>
+        <v>345096.61097773432</v>
+      </c>
+      <c r="L45" s="44">
+        <f t="shared" si="25"/>
+        <v>8683053.2820441425</v>
+      </c>
+      <c r="M45" s="44" t="str">
+        <f t="shared" si="25"/>
         <v>-</v>
       </c>
-      <c r="L45" s="44" t="str">
-        <f>IF(COLUMN()-COLUMN($E$45)&gt;$B$29,"-",L23-L28-L33+IF(COLUMN()-COLUMN($E$45)=$B$29,L40+L42,0))</f>
+      <c r="N45" s="44" t="str">
+        <f t="shared" si="25"/>
         <v>-</v>
       </c>
-      <c r="M45" s="44" t="str">
-        <f>IF(COLUMN()-COLUMN($E$45)&gt;$B$29,"-",M23-M28-M33+IF(COLUMN()-COLUMN($E$45)=$B$29,M40+M42,0))</f>
-        <v>-</v>
-      </c>
-      <c r="N45" s="44" t="str">
-        <f>IF(COLUMN()-COLUMN($E$45)&gt;$B$29,"-",N23-N28-N33+IF(COLUMN()-COLUMN($E$45)=$B$29,N40+N42,0))</f>
-        <v>-</v>
-      </c>
       <c r="O45" s="45" t="str">
-        <f>IF(COLUMN()-COLUMN($E$45)&gt;$B$29,"-",O23-O28-O33+IF(COLUMN()-COLUMN($E$45)=$B$29,O40+O42,0))</f>
+        <f t="shared" si="25"/>
         <v>-</v>
       </c>
     </row>
@@ -3752,18 +2753,18 @@
         <v>0.02</v>
       </c>
       <c r="C47" s="20"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="73"/>
-      <c r="F47" s="74"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="74"/>
-      <c r="I47" s="74"/>
-      <c r="J47" s="74"/>
-      <c r="K47" s="74"/>
-      <c r="L47" s="74"/>
-      <c r="M47" s="74"/>
-      <c r="N47" s="74"/>
-      <c r="O47" s="74"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="65"/>
+      <c r="H47" s="65"/>
+      <c r="I47" s="65"/>
+      <c r="J47" s="65"/>
+      <c r="K47" s="65"/>
+      <c r="L47" s="65"/>
+      <c r="M47" s="65"/>
+      <c r="N47" s="65"/>
+      <c r="O47" s="65"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D48" s="2" t="s">
@@ -3772,7 +2773,7 @@
       <c r="E48" s="8"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D49" s="15"/>
       <c r="E49" s="46" t="s">
         <v>78</v>
@@ -3781,59 +2782,60 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B50" s="65"/>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B50" s="62"/>
       <c r="D50" s="5" t="s">
         <v>80</v>
       </c>
       <c r="E50" s="23">
         <f ca="1">IRR(OFFSET($E$44,0,0,1,$B$29+1))</f>
-        <v>4.768307771460556E-2</v>
+        <v>0.11149745321478521</v>
       </c>
       <c r="F50" s="24">
         <f ca="1">IRR(OFFSET($E$45,0,0,1,$B$29+1))</f>
-        <v>3.5669658125026649E-2</v>
-      </c>
-      <c r="H50" s="55"/>
-      <c r="I50" s="55"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.18272178550664875</v>
+      </c>
+      <c r="H50" s="52"/>
+      <c r="I50" s="52"/>
+      <c r="L50" s="67"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D51" s="5" t="s">
         <v>81</v>
       </c>
       <c r="E51" s="48">
         <f ca="1">SUM(OFFSET($F$44,0,0,1,$B$29))/-$E$44</f>
-        <v>1.2423416512462433</v>
+        <v>1.9049054939433425</v>
       </c>
       <c r="F51" s="49">
         <f ca="1">SUM(OFFSET($F$45,0,0,1,$B$29))/-$E$45</f>
-        <v>1.18965069398839</v>
-      </c>
-      <c r="H51" s="55"/>
-      <c r="I51" s="55"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.8344597252082675</v>
+      </c>
+      <c r="H51" s="52"/>
+      <c r="I51" s="52"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D52" s="13" t="s">
         <v>82</v>
       </c>
       <c r="E52" s="38">
         <f ca="1">SUM(OFFSET(E44,0,0,1,$B$29+1))</f>
-        <v>2471884.8427116815</v>
+        <v>9230036.0382220969</v>
       </c>
       <c r="F52" s="39">
         <f ca="1">SUM(OFFSET(E45,0,0,1,$B$29+1))</f>
-        <v>701707.56775704306</v>
-      </c>
-      <c r="H52" s="64"/>
-      <c r="I52" s="64"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="55"/>
-      <c r="C53" s="56"/>
-      <c r="H53" s="64"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F56" s="55"/>
+        <v>6787500.9832705893</v>
+      </c>
+      <c r="H52" s="61"/>
+      <c r="I52" s="61"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" s="52"/>
+      <c r="C53" s="53"/>
+      <c r="H53" s="61"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F56" s="52"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>